<commit_message>
Arquivos modificados antes da gravação
</commit_message>
<xml_diff>
--- a/transacoes.xlsx
+++ b/transacoes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://overdax-my.sharepoint.com/personal/alison_pezzott_fluentebi_com/Documents/projetos/conversoes-moedas/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{5DEE88DF-BDDF-4ECC-85AE-143AEECC4204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{33893181-ABF4-40A1-9C22-DCC2A05D02FD}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{5DEE88DF-BDDF-4ECC-85AE-143AEECC4204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB24485B-59A9-4C7E-9E62-370BDB80A7BC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{852B7DE8-F81F-4112-B186-ED9A99A5D63B}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11055" xr2:uid="{852B7DE8-F81F-4112-B186-ED9A99A5D63B}"/>
   </bookViews>
   <sheets>
     <sheet name="Reais" sheetId="1" r:id="rId1"/>
@@ -72,7 +72,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -572,11 +572,11 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -635,30 +635,6 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="9"/>
-        <color theme="0"/>
-        <name val="Segoe UI"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
         <sz val="11"/>
         <color auto="1"/>
         <name val="Calibri"/>
@@ -689,7 +665,7 @@
         <family val="2"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+      <numFmt numFmtId="164" formatCode="#,##0.0000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -747,7 +723,31 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="#,##0.0000"/>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="9"/>
+        <color theme="0"/>
+        <name val="Segoe UI"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="#,##0.0000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
@@ -770,7 +770,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{91A40863-3D0E-4702-943F-0C0EC70D6E06}" name="fCotacoesReais" displayName="fCotacoesReais" ref="A1:D1001" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{91A40863-3D0E-4702-943F-0C0EC70D6E06}" name="fTransacoesReais" displayName="fTransacoesReais" ref="A1:D1001" totalsRowShown="0">
   <autoFilter ref="A1:D1001" xr:uid="{91A40863-3D0E-4702-943F-0C0EC70D6E06}"/>
   <tableColumns count="4">
     <tableColumn id="4" xr3:uid="{D72A4FC1-61F6-46FD-82CC-7C89ED4E4AEA}" name="ID"/>
@@ -783,13 +783,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B397A6F-4209-4F2A-A6B9-4E194D67E0DE}" name="fCotacoesSemConversao" displayName="fCotacoesSemConversao" ref="A1:D1001" totalsRowShown="0" headerRowDxfId="0" headerRowCellStyle="Normal 2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{4B397A6F-4209-4F2A-A6B9-4E194D67E0DE}" name="fTransacoesSemConversao" displayName="fTransacoesSemConversao" ref="A1:D1001" totalsRowShown="0" headerRowDxfId="4" headerRowCellStyle="Normal 2">
   <autoFilter ref="A1:D1001" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{C59EFE45-21C4-4F7C-8AE7-B44097056F9A}" name="ID" dataDxfId="4" dataCellStyle="Normal 2"/>
-    <tableColumn id="2" xr3:uid="{DEE16F9B-27B4-4355-BB24-35D03D574CED}" name="DataTransacao" dataDxfId="3" dataCellStyle="Normal 2"/>
-    <tableColumn id="3" xr3:uid="{D97DFC45-59DB-4585-81AF-5D73AB4F1ECA}" name="Total" dataDxfId="2" dataCellStyle="Normal 2"/>
-    <tableColumn id="4" xr3:uid="{0BECBADF-DCAC-41C6-8B22-5ED8FB7D9D7F}" name="Moeda" dataDxfId="1" dataCellStyle="Normal 2"/>
+    <tableColumn id="1" xr3:uid="{C59EFE45-21C4-4F7C-8AE7-B44097056F9A}" name="ID" dataDxfId="3" dataCellStyle="Normal 2"/>
+    <tableColumn id="2" xr3:uid="{DEE16F9B-27B4-4355-BB24-35D03D574CED}" name="DataTransacao" dataDxfId="2" dataCellStyle="Normal 2"/>
+    <tableColumn id="3" xr3:uid="{D97DFC45-59DB-4585-81AF-5D73AB4F1ECA}" name="Total" dataDxfId="1" dataCellStyle="Normal 2"/>
+    <tableColumn id="4" xr3:uid="{0BECBADF-DCAC-41C6-8B22-5ED8FB7D9D7F}" name="Moeda" dataDxfId="0" dataCellStyle="Normal 2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1114,7 +1114,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0E19D7D-8F23-4888-B448-0C2FF5AB85B1}">
   <dimension ref="A1:D1001"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -15151,7 +15153,7 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>